<commit_message>
Separated utils into a class module and a BLAST module Fixed various errors STABLE
</commit_message>
<xml_diff>
--- a/data/tables/Probes.xlsx
+++ b/data/tables/Probes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Archive\Trabajo\Profesiones\Bioinformática\PhD\Assignments\enERVate_v2\data\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6C888A80-0F07-44F2-B73F-9A9DFAD83667}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2173B455-D092-4940-AAB4-E0D4C6265232}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="810" yWindow="-120" windowWidth="19800" windowHeight="11760" xr2:uid="{5AD3A480-1531-467E-BA18-7A90A3BC149A}"/>
   </bookViews>
@@ -182,9 +182,6 @@
     <t>NP_789740.1</t>
   </si>
   <si>
-    <t>CAA40318A</t>
-  </si>
-  <si>
     <t>AFR79239.1</t>
   </si>
   <si>
@@ -399,6 +396,9 @@
   </si>
   <si>
     <t>M_protein</t>
+  </si>
+  <si>
+    <t>CAA40318.1</t>
   </si>
 </sst>
 </file>
@@ -773,7 +773,7 @@
   <dimension ref="A1:E58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D59" sqref="D59"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -802,7 +802,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -819,7 +819,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
@@ -836,7 +836,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
@@ -853,7 +853,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
@@ -870,7 +870,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B6" t="s">
         <v>8</v>
@@ -887,7 +887,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B7" t="s">
         <v>10</v>
@@ -904,7 +904,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B8" t="s">
         <v>12</v>
@@ -921,7 +921,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B9" t="s">
         <v>14</v>
@@ -938,7 +938,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B10" t="s">
         <v>16</v>
@@ -955,7 +955,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B11" t="s">
         <v>18</v>
@@ -972,7 +972,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B12" t="s">
         <v>20</v>
@@ -989,7 +989,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B13" t="s">
         <v>22</v>
@@ -1001,12 +1001,12 @@
         <v>36</v>
       </c>
       <c r="E13" t="s">
-        <v>48</v>
+        <v>120</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B14" t="s">
         <v>24</v>
@@ -1018,12 +1018,12 @@
         <v>36</v>
       </c>
       <c r="E14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B15" t="s">
         <v>26</v>
@@ -1035,7 +1035,7 @@
         <v>36</v>
       </c>
       <c r="E15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -1052,12 +1052,12 @@
         <v>36</v>
       </c>
       <c r="E16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B17" t="s">
         <v>0</v>
@@ -1066,15 +1066,15 @@
         <v>1</v>
       </c>
       <c r="D17" t="s">
+        <v>51</v>
+      </c>
+      <c r="E17" t="s">
         <v>52</v>
-      </c>
-      <c r="E17" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B18" t="s">
         <v>2</v>
@@ -1083,15 +1083,15 @@
         <v>3</v>
       </c>
       <c r="D18" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E18" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B19" t="s">
         <v>4</v>
@@ -1100,15 +1100,15 @@
         <v>5</v>
       </c>
       <c r="D19" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E19" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B20" t="s">
         <v>6</v>
@@ -1117,15 +1117,15 @@
         <v>7</v>
       </c>
       <c r="D20" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E20" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B21" t="s">
         <v>8</v>
@@ -1134,15 +1134,15 @@
         <v>9</v>
       </c>
       <c r="D21" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B22" t="s">
         <v>10</v>
@@ -1151,15 +1151,15 @@
         <v>11</v>
       </c>
       <c r="D22" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E22" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B23" t="s">
         <v>12</v>
@@ -1168,15 +1168,15 @@
         <v>13</v>
       </c>
       <c r="D23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E23" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B24" t="s">
         <v>14</v>
@@ -1185,15 +1185,15 @@
         <v>15</v>
       </c>
       <c r="D24" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E24" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B25" t="s">
         <v>16</v>
@@ -1202,15 +1202,15 @@
         <v>17</v>
       </c>
       <c r="D25" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B26" t="s">
         <v>18</v>
@@ -1219,15 +1219,15 @@
         <v>19</v>
       </c>
       <c r="D26" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E26" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B27" t="s">
         <v>20</v>
@@ -1236,15 +1236,15 @@
         <v>21</v>
       </c>
       <c r="D27" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E27" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B28" t="s">
         <v>22</v>
@@ -1253,15 +1253,15 @@
         <v>23</v>
       </c>
       <c r="D28" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E28" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B29" t="s">
         <v>24</v>
@@ -1270,15 +1270,15 @@
         <v>25</v>
       </c>
       <c r="D29" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E29" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B30" t="s">
         <v>26</v>
@@ -1287,10 +1287,10 @@
         <v>27</v>
       </c>
       <c r="D30" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E30" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -1304,15 +1304,15 @@
         <v>30</v>
       </c>
       <c r="D31" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E31" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B32" t="s">
         <v>0</v>
@@ -1321,15 +1321,15 @@
         <v>1</v>
       </c>
       <c r="D32" t="s">
+        <v>67</v>
+      </c>
+      <c r="E32" t="s">
         <v>68</v>
-      </c>
-      <c r="E32" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B33" t="s">
         <v>2</v>
@@ -1338,15 +1338,15 @@
         <v>3</v>
       </c>
       <c r="D33" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E33" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B34" t="s">
         <v>4</v>
@@ -1355,15 +1355,15 @@
         <v>5</v>
       </c>
       <c r="D34" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E34" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B35" t="s">
         <v>6</v>
@@ -1372,15 +1372,15 @@
         <v>7</v>
       </c>
       <c r="D35" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E35" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B36" t="s">
         <v>8</v>
@@ -1389,15 +1389,15 @@
         <v>9</v>
       </c>
       <c r="D36" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E36" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B37" t="s">
         <v>10</v>
@@ -1406,15 +1406,15 @@
         <v>11</v>
       </c>
       <c r="D37" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E37" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B38" t="s">
         <v>12</v>
@@ -1423,15 +1423,15 @@
         <v>13</v>
       </c>
       <c r="D38" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E38" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B39" t="s">
         <v>14</v>
@@ -1440,15 +1440,15 @@
         <v>15</v>
       </c>
       <c r="D39" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E39" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B40" t="s">
         <v>16</v>
@@ -1457,15 +1457,15 @@
         <v>17</v>
       </c>
       <c r="D40" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E40" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B41" t="s">
         <v>18</v>
@@ -1474,15 +1474,15 @@
         <v>19</v>
       </c>
       <c r="D41" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E41" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B42" t="s">
         <v>20</v>
@@ -1491,15 +1491,15 @@
         <v>21</v>
       </c>
       <c r="D42" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E42" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B43" t="s">
         <v>22</v>
@@ -1508,15 +1508,15 @@
         <v>23</v>
       </c>
       <c r="D43" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E43" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B44" t="s">
         <v>24</v>
@@ -1525,15 +1525,15 @@
         <v>25</v>
       </c>
       <c r="D44" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E44" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B45" t="s">
         <v>26</v>
@@ -1542,10 +1542,10 @@
         <v>27</v>
       </c>
       <c r="D45" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E45" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -1559,10 +1559,10 @@
         <v>30</v>
       </c>
       <c r="D46" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E46" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -1570,16 +1570,16 @@
         <v>28</v>
       </c>
       <c r="B47" t="s">
+        <v>83</v>
+      </c>
+      <c r="C47" t="s">
         <v>84</v>
       </c>
-      <c r="C47" t="s">
-        <v>85</v>
-      </c>
       <c r="D47" t="s">
+        <v>91</v>
+      </c>
+      <c r="E47" t="s">
         <v>92</v>
-      </c>
-      <c r="E47" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -1593,10 +1593,10 @@
         <v>21</v>
       </c>
       <c r="D48" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E48" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -1604,16 +1604,16 @@
         <v>28</v>
       </c>
       <c r="B49" t="s">
+        <v>85</v>
+      </c>
+      <c r="C49" t="s">
         <v>86</v>
       </c>
-      <c r="C49" t="s">
-        <v>87</v>
-      </c>
       <c r="D49" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E49" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -1621,16 +1621,16 @@
         <v>28</v>
       </c>
       <c r="B50" t="s">
+        <v>87</v>
+      </c>
+      <c r="C50" t="s">
         <v>88</v>
       </c>
-      <c r="C50" t="s">
-        <v>89</v>
-      </c>
       <c r="D50" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E50" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -1638,16 +1638,16 @@
         <v>28</v>
       </c>
       <c r="B51" t="s">
+        <v>89</v>
+      </c>
+      <c r="C51" t="s">
         <v>90</v>
       </c>
-      <c r="C51" t="s">
+      <c r="D51" t="s">
         <v>91</v>
       </c>
-      <c r="D51" t="s">
-        <v>92</v>
-      </c>
       <c r="E51" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -1661,112 +1661,112 @@
         <v>23</v>
       </c>
       <c r="D52" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E52" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
+        <v>98</v>
+      </c>
+      <c r="B53" t="s">
         <v>99</v>
       </c>
-      <c r="B53" t="s">
+      <c r="C53" t="s">
+        <v>106</v>
+      </c>
+      <c r="D53" t="s">
+        <v>114</v>
+      </c>
+      <c r="E53" t="s">
         <v>100</v>
-      </c>
-      <c r="C53" t="s">
-        <v>107</v>
-      </c>
-      <c r="D53" t="s">
-        <v>115</v>
-      </c>
-      <c r="E53" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
+        <v>98</v>
+      </c>
+      <c r="B54" t="s">
         <v>99</v>
       </c>
-      <c r="B54" t="s">
-        <v>100</v>
-      </c>
       <c r="C54" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D54" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E54" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
+        <v>98</v>
+      </c>
+      <c r="B55" t="s">
         <v>99</v>
       </c>
-      <c r="B55" t="s">
-        <v>100</v>
-      </c>
       <c r="C55" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D55" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E55" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
+        <v>98</v>
+      </c>
+      <c r="B56" t="s">
         <v>99</v>
       </c>
-      <c r="B56" t="s">
-        <v>100</v>
-      </c>
       <c r="C56" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D56" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E56" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
+        <v>98</v>
+      </c>
+      <c r="B57" t="s">
         <v>99</v>
       </c>
-      <c r="B57" t="s">
-        <v>100</v>
-      </c>
       <c r="C57" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D57" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E57" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
+        <v>98</v>
+      </c>
+      <c r="B58" t="s">
         <v>99</v>
       </c>
-      <c r="B58" t="s">
-        <v>100</v>
-      </c>
       <c r="C58" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D58" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E58" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>